<commit_message>
Updated repository with latest changes
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,119 +452,652 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>中国</t>
+          <t>美国</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14723</v>
+        <v>13094</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>美国</t>
+          <t>日本</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20937</v>
+        <v>4756</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>日本</t>
+          <t>德国</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5065</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2021</v>
+        <v>2005</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>中国</t>
+          <t>英国</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17734</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2021</v>
+        <v>2005</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>美国</t>
+          <t>中国</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23315</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2021</v>
+        <v>2005</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>日本</t>
+          <t>法国</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4937</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2022</v>
+        <v>2005</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>中国</t>
+          <t>意大利</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18100</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2022</v>
+        <v>2005</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>美国</t>
+          <t>加拿大</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25035</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2022</v>
+        <v>2005</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>西班牙</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>韩国</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>美国</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>14964</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>中国</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5812</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>日本</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>4231</v>
+      <c r="C14" t="n">
+        <v>5793</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>德国</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>法国</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>巴西</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>意大利</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>印度</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>俄罗斯</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>美国</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>18037</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>中国</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>11226</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>日本</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>德国</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>法国</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>印度</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>意大利</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>巴西</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>加拿大</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>美国</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>21323</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>中国</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>14688</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>日本</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>5056</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>德国</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>3888</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>印度</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2675</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>法国</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>意大利</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>加拿大</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>韩国</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>美国</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>28780</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>中国</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>18530</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>德国</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>日本</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>4110</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>印度</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>法国</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>意大利</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>巴西</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>加拿大</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>2240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>